<commit_message>
more M4S and MIP work
</commit_message>
<xml_diff>
--- a/Codes/MATLAB/POLYFEM/M4S_MIP_Boundary_Testing.xlsx
+++ b/Codes/MATLAB/POLYFEM/M4S_MIP_Boundary_Testing.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhackemack\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="M4S" sheetId="1" r:id="rId1"/>
+    <sheet name="MIP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="14">
   <si>
     <t>Method</t>
   </si>
@@ -64,12 +65,15 @@
   <si>
     <t>MIP</t>
   </si>
+  <si>
+    <t>triangles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +81,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,19 +135,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -133,8 +194,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3234796" cy="250453"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -177,6 +238,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -390,7 +452,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -433,6 +495,361 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝛼(𝑏,𝜙)−𝛾(𝑏,𝐷 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜕_𝑛 𝜙)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>−𝛽(𝐷 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜕_𝑛 𝑏</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>,𝜙)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3234796" cy="250453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="266700" y="85725"/>
+              <a:ext cx="3234796" cy="250453"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝛼</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>,</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜙</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝛾</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>,</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐷</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜕</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜙</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝛽</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐷</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> </m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜕</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>,</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜙</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="266700" y="85725"/>
+              <a:ext cx="3234796" cy="250453"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -739,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G19"/>
+  <dimension ref="A4:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,347 +1192,404 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>0.25</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="D5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>0.25</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="D6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>0.25</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
         <v>100</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>0.25</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="7">
         <v>0.25</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>0.25</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
         <v>100</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="C12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="C13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>100</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="1">
-        <v>10</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
         <v>100</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>10</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
         <v>100</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1124,4 +1598,185 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="15.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>100</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>